<commit_message>
Day 7 - extras
</commit_message>
<xml_diff>
--- a/Day07/day7.xlsx
+++ b/Day07/day7.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tesco-my.sharepoint.com/personal/craig_roberts_tesco_com/Documents/Dev/AdventOfCode/2021/Day07/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7ACDD162-B1C2-E945-9F9D-331A0FEE2889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="8_{7ACDD162-B1C2-E945-9F9D-331A0FEE2889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51E3DA1C-06B2-6E49-942D-A802C4AD7F92}"/>
   <bookViews>
-    <workbookView xWindow="16980" yWindow="-8980" windowWidth="38360" windowHeight="8980" xr2:uid="{769ADCBC-583A-F642-9D10-A13450553DD7}"/>
+    <workbookView xWindow="16980" yWindow="-8980" windowWidth="38360" windowHeight="8980" activeTab="1" xr2:uid="{769ADCBC-583A-F642-9D10-A13450553DD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="inspired" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,9 +34,17 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>length</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -57,8 +66,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -81,6 +97,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -96,7 +118,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -108,6 +130,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -428,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96F86573-2C3E-E04D-9590-625085372702}">
   <dimension ref="B2:S13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -645,4 +673,175 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCEE4C80-1D63-FE4E-8CFB-3F29A50D8910}">
+  <dimension ref="A2:R8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="18" width="4.83203125" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B2" s="5">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5">
+        <v>2</v>
+      </c>
+      <c r="E2" s="5">
+        <v>3</v>
+      </c>
+      <c r="F2" s="5">
+        <v>4</v>
+      </c>
+      <c r="G2" s="5">
+        <v>5</v>
+      </c>
+      <c r="H2" s="5">
+        <v>6</v>
+      </c>
+      <c r="I2" s="5">
+        <v>7</v>
+      </c>
+      <c r="J2" s="5">
+        <v>8</v>
+      </c>
+      <c r="K2" s="5">
+        <v>9</v>
+      </c>
+      <c r="L2" s="5">
+        <v>10</v>
+      </c>
+      <c r="M2" s="5">
+        <v>11</v>
+      </c>
+      <c r="N2" s="5">
+        <v>12</v>
+      </c>
+      <c r="O2" s="5">
+        <v>13</v>
+      </c>
+      <c r="P2" s="5">
+        <v>14</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>15</v>
+      </c>
+      <c r="R2" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="6"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B4" s="5"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>2</v>
+      </c>
+      <c r="H7" s="1">
+        <v>4</v>
+      </c>
+      <c r="I7" s="1">
+        <v>7</v>
+      </c>
+      <c r="J7" s="1">
+        <v>14</v>
+      </c>
+      <c r="K7" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
+        <f>COUNTA(B7:K7)</f>
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>